<commit_message>
Updated everything.qmd file. Rerendered.
</commit_message>
<xml_diff>
--- a/summary_file_FY2022_withTotals.xlsx
+++ b/summary_file_FY2022_withTotals.xlsx
@@ -6656,7 +6656,7 @@
         <v>3</v>
       </c>
       <c r="C554" t="n">
-        <v>2700.15</v>
+        <v>2700.24</v>
       </c>
     </row>
     <row r="555">
@@ -6777,7 +6777,7 @@
         <v>14</v>
       </c>
       <c r="C565" t="n">
-        <v>1879.05</v>
+        <v>1886.19</v>
       </c>
     </row>
     <row r="566">
@@ -6898,7 +6898,7 @@
         <v>25</v>
       </c>
       <c r="C576" t="n">
-        <v>104536.91</v>
+        <v>104544.13</v>
       </c>
     </row>
   </sheetData>
@@ -16075,10 +16075,10 @@
         <v>1.9</v>
       </c>
       <c r="C11" t="n">
-        <v>-4.68</v>
+        <v>-4.32</v>
       </c>
       <c r="D11" t="n">
-        <v>7.87</v>
+        <v>7.89</v>
       </c>
     </row>
     <row r="12">
@@ -16257,7 +16257,7 @@
         <v>104.5</v>
       </c>
       <c r="C24" t="n">
-        <v>14.15</v>
+        <v>14.16</v>
       </c>
       <c r="D24" t="n">
         <v>5.16</v>
@@ -16535,22 +16535,22 @@
         <v>14</v>
       </c>
       <c r="B12" t="n">
-        <v>-4.68</v>
+        <v>-4.32</v>
       </c>
       <c r="C12" t="n">
-        <v>15.06</v>
+        <v>15.28</v>
       </c>
       <c r="D12" t="n">
-        <v>16.83</v>
+        <v>16.98</v>
       </c>
       <c r="E12" t="n">
-        <v>9.26</v>
+        <v>9.34</v>
       </c>
       <c r="F12" t="n">
-        <v>6.23</v>
+        <v>6.27</v>
       </c>
       <c r="G12" t="n">
-        <v>7.87</v>
+        <v>7.89</v>
       </c>
     </row>
     <row r="13">
@@ -16800,7 +16800,7 @@
         <v>8.08</v>
       </c>
       <c r="F23" t="n">
-        <v>6.28</v>
+        <v>6.29</v>
       </c>
       <c r="G23" t="n">
         <v>4.54</v>
@@ -16811,13 +16811,13 @@
         <v>25</v>
       </c>
       <c r="B24" t="n">
-        <v>14.15</v>
+        <v>14.16</v>
       </c>
       <c r="C24" t="n">
         <v>18.36</v>
       </c>
       <c r="D24" t="n">
-        <v>13.15</v>
+        <v>13.16</v>
       </c>
       <c r="E24" t="n">
         <v>11.4</v>
@@ -17951,10 +17951,10 @@
         <v>101829.10187407</v>
       </c>
       <c r="C26" t="n">
-        <v>113021.56536341</v>
+        <v>113028.79108577</v>
       </c>
       <c r="D26" t="n">
-        <v>11192</v>
+        <v>11200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>